<commit_message>
Update APPlot for 4 Node Example
</commit_message>
<xml_diff>
--- a/4_Node_Heart_Network_Example.xlsx
+++ b/4_Node_Heart_Network_Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfen801\HeartModelPub\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfen801\HeartModelPub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08EEB45D-DAD3-4316-BA6E-6569B75FD02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3C45D7-3F22-4092-B10C-08DAC3200700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{CE794E2E-EB70-449E-A900-ACEA4681AAAE}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CE794E2E-EB70-449E-A900-ACEA4681AAAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Node" sheetId="1" r:id="rId1"/>
@@ -720,6 +720,29 @@
           <cell r="X2">
             <v>0.5</v>
           </cell>
+          <cell r="Y2"/>
+          <cell r="Z2"/>
+          <cell r="AA2"/>
+          <cell r="AB2"/>
+          <cell r="AC2"/>
+          <cell r="AD2"/>
+          <cell r="AE2"/>
+          <cell r="AF2"/>
+          <cell r="AG2"/>
+          <cell r="AH2"/>
+          <cell r="AI2"/>
+          <cell r="AJ2"/>
+          <cell r="AK2"/>
+          <cell r="AL2"/>
+          <cell r="AM2"/>
+          <cell r="AN2"/>
+          <cell r="AO2"/>
+          <cell r="AP2"/>
+          <cell r="AQ2"/>
+          <cell r="AR2"/>
+          <cell r="AS2"/>
+          <cell r="AT2"/>
+          <cell r="AU2"/>
           <cell r="AV2">
             <v>54.2</v>
           </cell>
@@ -737,6 +760,27 @@
           <cell r="C3">
             <v>2</v>
           </cell>
+          <cell r="D3"/>
+          <cell r="E3"/>
+          <cell r="F3"/>
+          <cell r="G3"/>
+          <cell r="H3"/>
+          <cell r="I3"/>
+          <cell r="J3"/>
+          <cell r="K3"/>
+          <cell r="L3"/>
+          <cell r="M3"/>
+          <cell r="N3"/>
+          <cell r="O3"/>
+          <cell r="P3"/>
+          <cell r="Q3"/>
+          <cell r="R3"/>
+          <cell r="S3"/>
+          <cell r="T3"/>
+          <cell r="U3"/>
+          <cell r="V3"/>
+          <cell r="W3"/>
+          <cell r="X3"/>
           <cell r="Y3">
             <v>-0.103765168727061</v>
           </cell>
@@ -823,6 +867,27 @@
           <cell r="C4">
             <v>3</v>
           </cell>
+          <cell r="D4"/>
+          <cell r="E4"/>
+          <cell r="F4"/>
+          <cell r="G4"/>
+          <cell r="H4"/>
+          <cell r="I4"/>
+          <cell r="J4"/>
+          <cell r="K4"/>
+          <cell r="L4"/>
+          <cell r="M4"/>
+          <cell r="N4"/>
+          <cell r="O4"/>
+          <cell r="P4"/>
+          <cell r="Q4"/>
+          <cell r="R4"/>
+          <cell r="S4"/>
+          <cell r="T4"/>
+          <cell r="U4"/>
+          <cell r="V4"/>
+          <cell r="W4"/>
+          <cell r="X4"/>
           <cell r="Y4">
             <v>-0.103765168727061</v>
           </cell>
@@ -909,6 +974,27 @@
           <cell r="C5">
             <v>4</v>
           </cell>
+          <cell r="D5"/>
+          <cell r="E5"/>
+          <cell r="F5"/>
+          <cell r="G5"/>
+          <cell r="H5"/>
+          <cell r="I5"/>
+          <cell r="J5"/>
+          <cell r="K5"/>
+          <cell r="L5"/>
+          <cell r="M5"/>
+          <cell r="N5"/>
+          <cell r="O5"/>
+          <cell r="P5"/>
+          <cell r="Q5"/>
+          <cell r="R5"/>
+          <cell r="S5"/>
+          <cell r="T5"/>
+          <cell r="U5"/>
+          <cell r="V5"/>
+          <cell r="W5"/>
+          <cell r="X5"/>
           <cell r="Y5">
             <v>-0.103765168727061</v>
           </cell>
@@ -1144,6 +1230,27 @@
           <cell r="C7">
             <v>6</v>
           </cell>
+          <cell r="D7"/>
+          <cell r="E7"/>
+          <cell r="F7"/>
+          <cell r="G7"/>
+          <cell r="H7"/>
+          <cell r="I7"/>
+          <cell r="J7"/>
+          <cell r="K7"/>
+          <cell r="L7"/>
+          <cell r="M7"/>
+          <cell r="N7"/>
+          <cell r="O7"/>
+          <cell r="P7"/>
+          <cell r="Q7"/>
+          <cell r="R7"/>
+          <cell r="S7"/>
+          <cell r="T7"/>
+          <cell r="U7"/>
+          <cell r="V7"/>
+          <cell r="W7"/>
+          <cell r="X7"/>
           <cell r="Y7">
             <v>-0.103765168727061</v>
           </cell>
@@ -1591,6 +1698,29 @@
           <cell r="X10">
             <v>0.5</v>
           </cell>
+          <cell r="Y10"/>
+          <cell r="Z10"/>
+          <cell r="AA10"/>
+          <cell r="AB10"/>
+          <cell r="AC10"/>
+          <cell r="AD10"/>
+          <cell r="AE10"/>
+          <cell r="AF10"/>
+          <cell r="AG10"/>
+          <cell r="AH10"/>
+          <cell r="AI10"/>
+          <cell r="AJ10"/>
+          <cell r="AK10"/>
+          <cell r="AL10"/>
+          <cell r="AM10"/>
+          <cell r="AN10"/>
+          <cell r="AO10"/>
+          <cell r="AP10"/>
+          <cell r="AQ10"/>
+          <cell r="AR10"/>
+          <cell r="AS10"/>
+          <cell r="AT10"/>
+          <cell r="AU10"/>
           <cell r="AV10">
             <v>60.2</v>
           </cell>
@@ -1969,6 +2099,29 @@
           <cell r="X13">
             <v>0.5</v>
           </cell>
+          <cell r="Y13"/>
+          <cell r="Z13"/>
+          <cell r="AA13"/>
+          <cell r="AB13"/>
+          <cell r="AC13"/>
+          <cell r="AD13"/>
+          <cell r="AE13"/>
+          <cell r="AF13"/>
+          <cell r="AG13"/>
+          <cell r="AH13"/>
+          <cell r="AI13"/>
+          <cell r="AJ13"/>
+          <cell r="AK13"/>
+          <cell r="AL13"/>
+          <cell r="AM13"/>
+          <cell r="AN13"/>
+          <cell r="AO13"/>
+          <cell r="AP13"/>
+          <cell r="AQ13"/>
+          <cell r="AR13"/>
+          <cell r="AS13"/>
+          <cell r="AT13"/>
+          <cell r="AU13"/>
           <cell r="AV13">
             <v>67.400000000000006</v>
           </cell>
@@ -1986,6 +2139,27 @@
           <cell r="C14">
             <v>13</v>
           </cell>
+          <cell r="D14"/>
+          <cell r="E14"/>
+          <cell r="F14"/>
+          <cell r="G14"/>
+          <cell r="H14"/>
+          <cell r="I14"/>
+          <cell r="J14"/>
+          <cell r="K14"/>
+          <cell r="L14"/>
+          <cell r="M14"/>
+          <cell r="N14"/>
+          <cell r="O14"/>
+          <cell r="P14"/>
+          <cell r="Q14"/>
+          <cell r="R14"/>
+          <cell r="S14"/>
+          <cell r="T14"/>
+          <cell r="U14"/>
+          <cell r="V14"/>
+          <cell r="W14"/>
+          <cell r="X14"/>
           <cell r="Y14">
             <v>-0.103765168727061</v>
           </cell>
@@ -2072,6 +2246,27 @@
           <cell r="C15">
             <v>14</v>
           </cell>
+          <cell r="D15"/>
+          <cell r="E15"/>
+          <cell r="F15"/>
+          <cell r="G15"/>
+          <cell r="H15"/>
+          <cell r="I15"/>
+          <cell r="J15"/>
+          <cell r="K15"/>
+          <cell r="L15"/>
+          <cell r="M15"/>
+          <cell r="N15"/>
+          <cell r="O15"/>
+          <cell r="P15"/>
+          <cell r="Q15"/>
+          <cell r="R15"/>
+          <cell r="S15"/>
+          <cell r="T15"/>
+          <cell r="U15"/>
+          <cell r="V15"/>
+          <cell r="W15"/>
+          <cell r="X15"/>
           <cell r="Y15">
             <v>-0.103765168727061</v>
           </cell>
@@ -2307,6 +2502,27 @@
           <cell r="C17">
             <v>16</v>
           </cell>
+          <cell r="D17"/>
+          <cell r="E17"/>
+          <cell r="F17"/>
+          <cell r="G17"/>
+          <cell r="H17"/>
+          <cell r="I17"/>
+          <cell r="J17"/>
+          <cell r="K17"/>
+          <cell r="L17"/>
+          <cell r="M17"/>
+          <cell r="N17"/>
+          <cell r="O17"/>
+          <cell r="P17"/>
+          <cell r="Q17"/>
+          <cell r="R17"/>
+          <cell r="S17"/>
+          <cell r="T17"/>
+          <cell r="U17"/>
+          <cell r="V17"/>
+          <cell r="W17"/>
+          <cell r="X17"/>
           <cell r="Y17">
             <v>-0.103765168727061</v>
           </cell>
@@ -2393,6 +2609,27 @@
           <cell r="C18">
             <v>17</v>
           </cell>
+          <cell r="D18"/>
+          <cell r="E18"/>
+          <cell r="F18"/>
+          <cell r="G18"/>
+          <cell r="H18"/>
+          <cell r="I18"/>
+          <cell r="J18"/>
+          <cell r="K18"/>
+          <cell r="L18"/>
+          <cell r="M18"/>
+          <cell r="N18"/>
+          <cell r="O18"/>
+          <cell r="P18"/>
+          <cell r="Q18"/>
+          <cell r="R18"/>
+          <cell r="S18"/>
+          <cell r="T18"/>
+          <cell r="U18"/>
+          <cell r="V18"/>
+          <cell r="W18"/>
+          <cell r="X18"/>
           <cell r="Y18">
             <v>-0.103765168727061</v>
           </cell>
@@ -2479,6 +2716,27 @@
           <cell r="C19">
             <v>18</v>
           </cell>
+          <cell r="D19"/>
+          <cell r="E19"/>
+          <cell r="F19"/>
+          <cell r="G19"/>
+          <cell r="H19"/>
+          <cell r="I19"/>
+          <cell r="J19"/>
+          <cell r="K19"/>
+          <cell r="L19"/>
+          <cell r="M19"/>
+          <cell r="N19"/>
+          <cell r="O19"/>
+          <cell r="P19"/>
+          <cell r="Q19"/>
+          <cell r="R19"/>
+          <cell r="S19"/>
+          <cell r="T19"/>
+          <cell r="U19"/>
+          <cell r="V19"/>
+          <cell r="W19"/>
+          <cell r="X19"/>
           <cell r="Y19">
             <v>-0.103765168727061</v>
           </cell>
@@ -4055,6 +4313,27 @@
           <cell r="C30">
             <v>29</v>
           </cell>
+          <cell r="D30"/>
+          <cell r="E30"/>
+          <cell r="F30"/>
+          <cell r="G30"/>
+          <cell r="H30"/>
+          <cell r="I30"/>
+          <cell r="J30"/>
+          <cell r="K30"/>
+          <cell r="L30"/>
+          <cell r="M30"/>
+          <cell r="N30"/>
+          <cell r="O30"/>
+          <cell r="P30"/>
+          <cell r="Q30"/>
+          <cell r="R30"/>
+          <cell r="S30"/>
+          <cell r="T30"/>
+          <cell r="U30"/>
+          <cell r="V30"/>
+          <cell r="W30"/>
+          <cell r="X30"/>
           <cell r="Y30">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4141,6 +4420,27 @@
           <cell r="C31">
             <v>30</v>
           </cell>
+          <cell r="D31"/>
+          <cell r="E31"/>
+          <cell r="F31"/>
+          <cell r="G31"/>
+          <cell r="H31"/>
+          <cell r="I31"/>
+          <cell r="J31"/>
+          <cell r="K31"/>
+          <cell r="L31"/>
+          <cell r="M31"/>
+          <cell r="N31"/>
+          <cell r="O31"/>
+          <cell r="P31"/>
+          <cell r="Q31"/>
+          <cell r="R31"/>
+          <cell r="S31"/>
+          <cell r="T31"/>
+          <cell r="U31"/>
+          <cell r="V31"/>
+          <cell r="W31"/>
+          <cell r="X31"/>
           <cell r="Y31">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4227,6 +4527,27 @@
           <cell r="C32">
             <v>31</v>
           </cell>
+          <cell r="D32"/>
+          <cell r="E32"/>
+          <cell r="F32"/>
+          <cell r="G32"/>
+          <cell r="H32"/>
+          <cell r="I32"/>
+          <cell r="J32"/>
+          <cell r="K32"/>
+          <cell r="L32"/>
+          <cell r="M32"/>
+          <cell r="N32"/>
+          <cell r="O32"/>
+          <cell r="P32"/>
+          <cell r="Q32"/>
+          <cell r="R32"/>
+          <cell r="S32"/>
+          <cell r="T32"/>
+          <cell r="U32"/>
+          <cell r="V32"/>
+          <cell r="W32"/>
+          <cell r="X32"/>
           <cell r="Y32">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4313,6 +4634,27 @@
           <cell r="C33">
             <v>32</v>
           </cell>
+          <cell r="D33"/>
+          <cell r="E33"/>
+          <cell r="F33"/>
+          <cell r="G33"/>
+          <cell r="H33"/>
+          <cell r="I33"/>
+          <cell r="J33"/>
+          <cell r="K33"/>
+          <cell r="L33"/>
+          <cell r="M33"/>
+          <cell r="N33"/>
+          <cell r="O33"/>
+          <cell r="P33"/>
+          <cell r="Q33"/>
+          <cell r="R33"/>
+          <cell r="S33"/>
+          <cell r="T33"/>
+          <cell r="U33"/>
+          <cell r="V33"/>
+          <cell r="W33"/>
+          <cell r="X33"/>
           <cell r="Y33">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4697,6 +5039,27 @@
           <cell r="C36">
             <v>35</v>
           </cell>
+          <cell r="D36"/>
+          <cell r="E36"/>
+          <cell r="F36"/>
+          <cell r="G36"/>
+          <cell r="H36"/>
+          <cell r="I36"/>
+          <cell r="J36"/>
+          <cell r="K36"/>
+          <cell r="L36"/>
+          <cell r="M36"/>
+          <cell r="N36"/>
+          <cell r="O36"/>
+          <cell r="P36"/>
+          <cell r="Q36"/>
+          <cell r="R36"/>
+          <cell r="S36"/>
+          <cell r="T36"/>
+          <cell r="U36"/>
+          <cell r="V36"/>
+          <cell r="W36"/>
+          <cell r="X36"/>
           <cell r="Y36">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4783,6 +5146,27 @@
           <cell r="C37">
             <v>36</v>
           </cell>
+          <cell r="D37"/>
+          <cell r="E37"/>
+          <cell r="F37"/>
+          <cell r="G37"/>
+          <cell r="H37"/>
+          <cell r="I37"/>
+          <cell r="J37"/>
+          <cell r="K37"/>
+          <cell r="L37"/>
+          <cell r="M37"/>
+          <cell r="N37"/>
+          <cell r="O37"/>
+          <cell r="P37"/>
+          <cell r="Q37"/>
+          <cell r="R37"/>
+          <cell r="S37"/>
+          <cell r="T37"/>
+          <cell r="U37"/>
+          <cell r="V37"/>
+          <cell r="W37"/>
+          <cell r="X37"/>
           <cell r="Y37">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4869,6 +5253,27 @@
           <cell r="C38">
             <v>37</v>
           </cell>
+          <cell r="D38"/>
+          <cell r="E38"/>
+          <cell r="F38"/>
+          <cell r="G38"/>
+          <cell r="H38"/>
+          <cell r="I38"/>
+          <cell r="J38"/>
+          <cell r="K38"/>
+          <cell r="L38"/>
+          <cell r="M38"/>
+          <cell r="N38"/>
+          <cell r="O38"/>
+          <cell r="P38"/>
+          <cell r="Q38"/>
+          <cell r="R38"/>
+          <cell r="S38"/>
+          <cell r="T38"/>
+          <cell r="U38"/>
+          <cell r="V38"/>
+          <cell r="W38"/>
+          <cell r="X38"/>
           <cell r="Y38">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5253,6 +5658,27 @@
           <cell r="C41">
             <v>40</v>
           </cell>
+          <cell r="D41"/>
+          <cell r="E41"/>
+          <cell r="F41"/>
+          <cell r="G41"/>
+          <cell r="H41"/>
+          <cell r="I41"/>
+          <cell r="J41"/>
+          <cell r="K41"/>
+          <cell r="L41"/>
+          <cell r="M41"/>
+          <cell r="N41"/>
+          <cell r="O41"/>
+          <cell r="P41"/>
+          <cell r="Q41"/>
+          <cell r="R41"/>
+          <cell r="S41"/>
+          <cell r="T41"/>
+          <cell r="U41"/>
+          <cell r="V41"/>
+          <cell r="W41"/>
+          <cell r="X41"/>
           <cell r="Y41">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5339,6 +5765,27 @@
           <cell r="C42">
             <v>41</v>
           </cell>
+          <cell r="D42"/>
+          <cell r="E42"/>
+          <cell r="F42"/>
+          <cell r="G42"/>
+          <cell r="H42"/>
+          <cell r="I42"/>
+          <cell r="J42"/>
+          <cell r="K42"/>
+          <cell r="L42"/>
+          <cell r="M42"/>
+          <cell r="N42"/>
+          <cell r="O42"/>
+          <cell r="P42"/>
+          <cell r="Q42"/>
+          <cell r="R42"/>
+          <cell r="S42"/>
+          <cell r="T42"/>
+          <cell r="U42"/>
+          <cell r="V42"/>
+          <cell r="W42"/>
+          <cell r="X42"/>
           <cell r="Y42">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5425,6 +5872,27 @@
           <cell r="C43">
             <v>42</v>
           </cell>
+          <cell r="D43"/>
+          <cell r="E43"/>
+          <cell r="F43"/>
+          <cell r="G43"/>
+          <cell r="H43"/>
+          <cell r="I43"/>
+          <cell r="J43"/>
+          <cell r="K43"/>
+          <cell r="L43"/>
+          <cell r="M43"/>
+          <cell r="N43"/>
+          <cell r="O43"/>
+          <cell r="P43"/>
+          <cell r="Q43"/>
+          <cell r="R43"/>
+          <cell r="S43"/>
+          <cell r="T43"/>
+          <cell r="U43"/>
+          <cell r="V43"/>
+          <cell r="W43"/>
+          <cell r="X43"/>
           <cell r="Y43">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5511,6 +5979,27 @@
           <cell r="C44">
             <v>43</v>
           </cell>
+          <cell r="D44"/>
+          <cell r="E44"/>
+          <cell r="F44"/>
+          <cell r="G44"/>
+          <cell r="H44"/>
+          <cell r="I44"/>
+          <cell r="J44"/>
+          <cell r="K44"/>
+          <cell r="L44"/>
+          <cell r="M44"/>
+          <cell r="N44"/>
+          <cell r="O44"/>
+          <cell r="P44"/>
+          <cell r="Q44"/>
+          <cell r="R44"/>
+          <cell r="S44"/>
+          <cell r="T44"/>
+          <cell r="U44"/>
+          <cell r="V44"/>
+          <cell r="W44"/>
+          <cell r="X44"/>
           <cell r="Y44">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5591,6 +6080,29 @@
           <cell r="A45" t="str">
             <v>REF</v>
           </cell>
+          <cell r="B45"/>
+          <cell r="C45"/>
+          <cell r="D45"/>
+          <cell r="E45"/>
+          <cell r="F45"/>
+          <cell r="G45"/>
+          <cell r="H45"/>
+          <cell r="I45"/>
+          <cell r="J45"/>
+          <cell r="K45"/>
+          <cell r="L45"/>
+          <cell r="M45"/>
+          <cell r="N45"/>
+          <cell r="O45"/>
+          <cell r="P45"/>
+          <cell r="Q45"/>
+          <cell r="R45"/>
+          <cell r="S45"/>
+          <cell r="T45"/>
+          <cell r="U45"/>
+          <cell r="V45"/>
+          <cell r="W45"/>
+          <cell r="X45"/>
           <cell r="Y45">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5645,6 +6157,11 @@
           <cell r="AP45">
             <v>131.1</v>
           </cell>
+          <cell r="AQ45"/>
+          <cell r="AR45"/>
+          <cell r="AS45"/>
+          <cell r="AT45"/>
+          <cell r="AU45"/>
           <cell r="AV45">
             <v>0</v>
           </cell>
@@ -5985,8 +6502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09EE518-A6B0-4237-BA56-0ADD842FBD35}">
   <dimension ref="A1:AZ5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6160,7 +6677,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="7">
-        <v>2.1</v>
+        <v>1.5</v>
       </c>
       <c r="E2" s="7">
         <v>2E-3</v>
@@ -6318,7 +6835,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="7">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="E3" s="7">
         <v>2E-3</v>
@@ -6476,7 +6993,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="7">
-        <v>2.2999999999999998</v>
+        <v>3</v>
       </c>
       <c r="E4" s="7">
         <v>2E-3</v>
@@ -6791,8 +7308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D028EE44-7DA0-4D5B-B019-D6C46FBDD67D}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Setup single case of reentry
</commit_message>
<xml_diff>
--- a/4_Node_Heart_Network_Example.xlsx
+++ b/4_Node_Heart_Network_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfen801\HeartModelPub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3C45D7-3F22-4092-B10C-08DAC3200700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA71B3A-B22E-452D-90F2-D7791B84A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{CE794E2E-EB70-449E-A900-ACEA4681AAAE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{CE794E2E-EB70-449E-A900-ACEA4681AAAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Node" sheetId="1" r:id="rId1"/>
@@ -720,29 +720,6 @@
           <cell r="X2">
             <v>0.5</v>
           </cell>
-          <cell r="Y2"/>
-          <cell r="Z2"/>
-          <cell r="AA2"/>
-          <cell r="AB2"/>
-          <cell r="AC2"/>
-          <cell r="AD2"/>
-          <cell r="AE2"/>
-          <cell r="AF2"/>
-          <cell r="AG2"/>
-          <cell r="AH2"/>
-          <cell r="AI2"/>
-          <cell r="AJ2"/>
-          <cell r="AK2"/>
-          <cell r="AL2"/>
-          <cell r="AM2"/>
-          <cell r="AN2"/>
-          <cell r="AO2"/>
-          <cell r="AP2"/>
-          <cell r="AQ2"/>
-          <cell r="AR2"/>
-          <cell r="AS2"/>
-          <cell r="AT2"/>
-          <cell r="AU2"/>
           <cell r="AV2">
             <v>54.2</v>
           </cell>
@@ -760,27 +737,6 @@
           <cell r="C3">
             <v>2</v>
           </cell>
-          <cell r="D3"/>
-          <cell r="E3"/>
-          <cell r="F3"/>
-          <cell r="G3"/>
-          <cell r="H3"/>
-          <cell r="I3"/>
-          <cell r="J3"/>
-          <cell r="K3"/>
-          <cell r="L3"/>
-          <cell r="M3"/>
-          <cell r="N3"/>
-          <cell r="O3"/>
-          <cell r="P3"/>
-          <cell r="Q3"/>
-          <cell r="R3"/>
-          <cell r="S3"/>
-          <cell r="T3"/>
-          <cell r="U3"/>
-          <cell r="V3"/>
-          <cell r="W3"/>
-          <cell r="X3"/>
           <cell r="Y3">
             <v>-0.103765168727061</v>
           </cell>
@@ -867,27 +823,6 @@
           <cell r="C4">
             <v>3</v>
           </cell>
-          <cell r="D4"/>
-          <cell r="E4"/>
-          <cell r="F4"/>
-          <cell r="G4"/>
-          <cell r="H4"/>
-          <cell r="I4"/>
-          <cell r="J4"/>
-          <cell r="K4"/>
-          <cell r="L4"/>
-          <cell r="M4"/>
-          <cell r="N4"/>
-          <cell r="O4"/>
-          <cell r="P4"/>
-          <cell r="Q4"/>
-          <cell r="R4"/>
-          <cell r="S4"/>
-          <cell r="T4"/>
-          <cell r="U4"/>
-          <cell r="V4"/>
-          <cell r="W4"/>
-          <cell r="X4"/>
           <cell r="Y4">
             <v>-0.103765168727061</v>
           </cell>
@@ -974,27 +909,6 @@
           <cell r="C5">
             <v>4</v>
           </cell>
-          <cell r="D5"/>
-          <cell r="E5"/>
-          <cell r="F5"/>
-          <cell r="G5"/>
-          <cell r="H5"/>
-          <cell r="I5"/>
-          <cell r="J5"/>
-          <cell r="K5"/>
-          <cell r="L5"/>
-          <cell r="M5"/>
-          <cell r="N5"/>
-          <cell r="O5"/>
-          <cell r="P5"/>
-          <cell r="Q5"/>
-          <cell r="R5"/>
-          <cell r="S5"/>
-          <cell r="T5"/>
-          <cell r="U5"/>
-          <cell r="V5"/>
-          <cell r="W5"/>
-          <cell r="X5"/>
           <cell r="Y5">
             <v>-0.103765168727061</v>
           </cell>
@@ -1230,27 +1144,6 @@
           <cell r="C7">
             <v>6</v>
           </cell>
-          <cell r="D7"/>
-          <cell r="E7"/>
-          <cell r="F7"/>
-          <cell r="G7"/>
-          <cell r="H7"/>
-          <cell r="I7"/>
-          <cell r="J7"/>
-          <cell r="K7"/>
-          <cell r="L7"/>
-          <cell r="M7"/>
-          <cell r="N7"/>
-          <cell r="O7"/>
-          <cell r="P7"/>
-          <cell r="Q7"/>
-          <cell r="R7"/>
-          <cell r="S7"/>
-          <cell r="T7"/>
-          <cell r="U7"/>
-          <cell r="V7"/>
-          <cell r="W7"/>
-          <cell r="X7"/>
           <cell r="Y7">
             <v>-0.103765168727061</v>
           </cell>
@@ -1698,29 +1591,6 @@
           <cell r="X10">
             <v>0.5</v>
           </cell>
-          <cell r="Y10"/>
-          <cell r="Z10"/>
-          <cell r="AA10"/>
-          <cell r="AB10"/>
-          <cell r="AC10"/>
-          <cell r="AD10"/>
-          <cell r="AE10"/>
-          <cell r="AF10"/>
-          <cell r="AG10"/>
-          <cell r="AH10"/>
-          <cell r="AI10"/>
-          <cell r="AJ10"/>
-          <cell r="AK10"/>
-          <cell r="AL10"/>
-          <cell r="AM10"/>
-          <cell r="AN10"/>
-          <cell r="AO10"/>
-          <cell r="AP10"/>
-          <cell r="AQ10"/>
-          <cell r="AR10"/>
-          <cell r="AS10"/>
-          <cell r="AT10"/>
-          <cell r="AU10"/>
           <cell r="AV10">
             <v>60.2</v>
           </cell>
@@ -2099,29 +1969,6 @@
           <cell r="X13">
             <v>0.5</v>
           </cell>
-          <cell r="Y13"/>
-          <cell r="Z13"/>
-          <cell r="AA13"/>
-          <cell r="AB13"/>
-          <cell r="AC13"/>
-          <cell r="AD13"/>
-          <cell r="AE13"/>
-          <cell r="AF13"/>
-          <cell r="AG13"/>
-          <cell r="AH13"/>
-          <cell r="AI13"/>
-          <cell r="AJ13"/>
-          <cell r="AK13"/>
-          <cell r="AL13"/>
-          <cell r="AM13"/>
-          <cell r="AN13"/>
-          <cell r="AO13"/>
-          <cell r="AP13"/>
-          <cell r="AQ13"/>
-          <cell r="AR13"/>
-          <cell r="AS13"/>
-          <cell r="AT13"/>
-          <cell r="AU13"/>
           <cell r="AV13">
             <v>67.400000000000006</v>
           </cell>
@@ -2139,27 +1986,6 @@
           <cell r="C14">
             <v>13</v>
           </cell>
-          <cell r="D14"/>
-          <cell r="E14"/>
-          <cell r="F14"/>
-          <cell r="G14"/>
-          <cell r="H14"/>
-          <cell r="I14"/>
-          <cell r="J14"/>
-          <cell r="K14"/>
-          <cell r="L14"/>
-          <cell r="M14"/>
-          <cell r="N14"/>
-          <cell r="O14"/>
-          <cell r="P14"/>
-          <cell r="Q14"/>
-          <cell r="R14"/>
-          <cell r="S14"/>
-          <cell r="T14"/>
-          <cell r="U14"/>
-          <cell r="V14"/>
-          <cell r="W14"/>
-          <cell r="X14"/>
           <cell r="Y14">
             <v>-0.103765168727061</v>
           </cell>
@@ -2246,27 +2072,6 @@
           <cell r="C15">
             <v>14</v>
           </cell>
-          <cell r="D15"/>
-          <cell r="E15"/>
-          <cell r="F15"/>
-          <cell r="G15"/>
-          <cell r="H15"/>
-          <cell r="I15"/>
-          <cell r="J15"/>
-          <cell r="K15"/>
-          <cell r="L15"/>
-          <cell r="M15"/>
-          <cell r="N15"/>
-          <cell r="O15"/>
-          <cell r="P15"/>
-          <cell r="Q15"/>
-          <cell r="R15"/>
-          <cell r="S15"/>
-          <cell r="T15"/>
-          <cell r="U15"/>
-          <cell r="V15"/>
-          <cell r="W15"/>
-          <cell r="X15"/>
           <cell r="Y15">
             <v>-0.103765168727061</v>
           </cell>
@@ -2502,27 +2307,6 @@
           <cell r="C17">
             <v>16</v>
           </cell>
-          <cell r="D17"/>
-          <cell r="E17"/>
-          <cell r="F17"/>
-          <cell r="G17"/>
-          <cell r="H17"/>
-          <cell r="I17"/>
-          <cell r="J17"/>
-          <cell r="K17"/>
-          <cell r="L17"/>
-          <cell r="M17"/>
-          <cell r="N17"/>
-          <cell r="O17"/>
-          <cell r="P17"/>
-          <cell r="Q17"/>
-          <cell r="R17"/>
-          <cell r="S17"/>
-          <cell r="T17"/>
-          <cell r="U17"/>
-          <cell r="V17"/>
-          <cell r="W17"/>
-          <cell r="X17"/>
           <cell r="Y17">
             <v>-0.103765168727061</v>
           </cell>
@@ -2609,27 +2393,6 @@
           <cell r="C18">
             <v>17</v>
           </cell>
-          <cell r="D18"/>
-          <cell r="E18"/>
-          <cell r="F18"/>
-          <cell r="G18"/>
-          <cell r="H18"/>
-          <cell r="I18"/>
-          <cell r="J18"/>
-          <cell r="K18"/>
-          <cell r="L18"/>
-          <cell r="M18"/>
-          <cell r="N18"/>
-          <cell r="O18"/>
-          <cell r="P18"/>
-          <cell r="Q18"/>
-          <cell r="R18"/>
-          <cell r="S18"/>
-          <cell r="T18"/>
-          <cell r="U18"/>
-          <cell r="V18"/>
-          <cell r="W18"/>
-          <cell r="X18"/>
           <cell r="Y18">
             <v>-0.103765168727061</v>
           </cell>
@@ -2716,27 +2479,6 @@
           <cell r="C19">
             <v>18</v>
           </cell>
-          <cell r="D19"/>
-          <cell r="E19"/>
-          <cell r="F19"/>
-          <cell r="G19"/>
-          <cell r="H19"/>
-          <cell r="I19"/>
-          <cell r="J19"/>
-          <cell r="K19"/>
-          <cell r="L19"/>
-          <cell r="M19"/>
-          <cell r="N19"/>
-          <cell r="O19"/>
-          <cell r="P19"/>
-          <cell r="Q19"/>
-          <cell r="R19"/>
-          <cell r="S19"/>
-          <cell r="T19"/>
-          <cell r="U19"/>
-          <cell r="V19"/>
-          <cell r="W19"/>
-          <cell r="X19"/>
           <cell r="Y19">
             <v>-0.103765168727061</v>
           </cell>
@@ -4313,27 +4055,6 @@
           <cell r="C30">
             <v>29</v>
           </cell>
-          <cell r="D30"/>
-          <cell r="E30"/>
-          <cell r="F30"/>
-          <cell r="G30"/>
-          <cell r="H30"/>
-          <cell r="I30"/>
-          <cell r="J30"/>
-          <cell r="K30"/>
-          <cell r="L30"/>
-          <cell r="M30"/>
-          <cell r="N30"/>
-          <cell r="O30"/>
-          <cell r="P30"/>
-          <cell r="Q30"/>
-          <cell r="R30"/>
-          <cell r="S30"/>
-          <cell r="T30"/>
-          <cell r="U30"/>
-          <cell r="V30"/>
-          <cell r="W30"/>
-          <cell r="X30"/>
           <cell r="Y30">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4420,27 +4141,6 @@
           <cell r="C31">
             <v>30</v>
           </cell>
-          <cell r="D31"/>
-          <cell r="E31"/>
-          <cell r="F31"/>
-          <cell r="G31"/>
-          <cell r="H31"/>
-          <cell r="I31"/>
-          <cell r="J31"/>
-          <cell r="K31"/>
-          <cell r="L31"/>
-          <cell r="M31"/>
-          <cell r="N31"/>
-          <cell r="O31"/>
-          <cell r="P31"/>
-          <cell r="Q31"/>
-          <cell r="R31"/>
-          <cell r="S31"/>
-          <cell r="T31"/>
-          <cell r="U31"/>
-          <cell r="V31"/>
-          <cell r="W31"/>
-          <cell r="X31"/>
           <cell r="Y31">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4527,27 +4227,6 @@
           <cell r="C32">
             <v>31</v>
           </cell>
-          <cell r="D32"/>
-          <cell r="E32"/>
-          <cell r="F32"/>
-          <cell r="G32"/>
-          <cell r="H32"/>
-          <cell r="I32"/>
-          <cell r="J32"/>
-          <cell r="K32"/>
-          <cell r="L32"/>
-          <cell r="M32"/>
-          <cell r="N32"/>
-          <cell r="O32"/>
-          <cell r="P32"/>
-          <cell r="Q32"/>
-          <cell r="R32"/>
-          <cell r="S32"/>
-          <cell r="T32"/>
-          <cell r="U32"/>
-          <cell r="V32"/>
-          <cell r="W32"/>
-          <cell r="X32"/>
           <cell r="Y32">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -4634,27 +4313,6 @@
           <cell r="C33">
             <v>32</v>
           </cell>
-          <cell r="D33"/>
-          <cell r="E33"/>
-          <cell r="F33"/>
-          <cell r="G33"/>
-          <cell r="H33"/>
-          <cell r="I33"/>
-          <cell r="J33"/>
-          <cell r="K33"/>
-          <cell r="L33"/>
-          <cell r="M33"/>
-          <cell r="N33"/>
-          <cell r="O33"/>
-          <cell r="P33"/>
-          <cell r="Q33"/>
-          <cell r="R33"/>
-          <cell r="S33"/>
-          <cell r="T33"/>
-          <cell r="U33"/>
-          <cell r="V33"/>
-          <cell r="W33"/>
-          <cell r="X33"/>
           <cell r="Y33">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5039,27 +4697,6 @@
           <cell r="C36">
             <v>35</v>
           </cell>
-          <cell r="D36"/>
-          <cell r="E36"/>
-          <cell r="F36"/>
-          <cell r="G36"/>
-          <cell r="H36"/>
-          <cell r="I36"/>
-          <cell r="J36"/>
-          <cell r="K36"/>
-          <cell r="L36"/>
-          <cell r="M36"/>
-          <cell r="N36"/>
-          <cell r="O36"/>
-          <cell r="P36"/>
-          <cell r="Q36"/>
-          <cell r="R36"/>
-          <cell r="S36"/>
-          <cell r="T36"/>
-          <cell r="U36"/>
-          <cell r="V36"/>
-          <cell r="W36"/>
-          <cell r="X36"/>
           <cell r="Y36">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5146,27 +4783,6 @@
           <cell r="C37">
             <v>36</v>
           </cell>
-          <cell r="D37"/>
-          <cell r="E37"/>
-          <cell r="F37"/>
-          <cell r="G37"/>
-          <cell r="H37"/>
-          <cell r="I37"/>
-          <cell r="J37"/>
-          <cell r="K37"/>
-          <cell r="L37"/>
-          <cell r="M37"/>
-          <cell r="N37"/>
-          <cell r="O37"/>
-          <cell r="P37"/>
-          <cell r="Q37"/>
-          <cell r="R37"/>
-          <cell r="S37"/>
-          <cell r="T37"/>
-          <cell r="U37"/>
-          <cell r="V37"/>
-          <cell r="W37"/>
-          <cell r="X37"/>
           <cell r="Y37">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5253,27 +4869,6 @@
           <cell r="C38">
             <v>37</v>
           </cell>
-          <cell r="D38"/>
-          <cell r="E38"/>
-          <cell r="F38"/>
-          <cell r="G38"/>
-          <cell r="H38"/>
-          <cell r="I38"/>
-          <cell r="J38"/>
-          <cell r="K38"/>
-          <cell r="L38"/>
-          <cell r="M38"/>
-          <cell r="N38"/>
-          <cell r="O38"/>
-          <cell r="P38"/>
-          <cell r="Q38"/>
-          <cell r="R38"/>
-          <cell r="S38"/>
-          <cell r="T38"/>
-          <cell r="U38"/>
-          <cell r="V38"/>
-          <cell r="W38"/>
-          <cell r="X38"/>
           <cell r="Y38">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5658,27 +5253,6 @@
           <cell r="C41">
             <v>40</v>
           </cell>
-          <cell r="D41"/>
-          <cell r="E41"/>
-          <cell r="F41"/>
-          <cell r="G41"/>
-          <cell r="H41"/>
-          <cell r="I41"/>
-          <cell r="J41"/>
-          <cell r="K41"/>
-          <cell r="L41"/>
-          <cell r="M41"/>
-          <cell r="N41"/>
-          <cell r="O41"/>
-          <cell r="P41"/>
-          <cell r="Q41"/>
-          <cell r="R41"/>
-          <cell r="S41"/>
-          <cell r="T41"/>
-          <cell r="U41"/>
-          <cell r="V41"/>
-          <cell r="W41"/>
-          <cell r="X41"/>
           <cell r="Y41">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5765,27 +5339,6 @@
           <cell r="C42">
             <v>41</v>
           </cell>
-          <cell r="D42"/>
-          <cell r="E42"/>
-          <cell r="F42"/>
-          <cell r="G42"/>
-          <cell r="H42"/>
-          <cell r="I42"/>
-          <cell r="J42"/>
-          <cell r="K42"/>
-          <cell r="L42"/>
-          <cell r="M42"/>
-          <cell r="N42"/>
-          <cell r="O42"/>
-          <cell r="P42"/>
-          <cell r="Q42"/>
-          <cell r="R42"/>
-          <cell r="S42"/>
-          <cell r="T42"/>
-          <cell r="U42"/>
-          <cell r="V42"/>
-          <cell r="W42"/>
-          <cell r="X42"/>
           <cell r="Y42">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5872,27 +5425,6 @@
           <cell r="C43">
             <v>42</v>
           </cell>
-          <cell r="D43"/>
-          <cell r="E43"/>
-          <cell r="F43"/>
-          <cell r="G43"/>
-          <cell r="H43"/>
-          <cell r="I43"/>
-          <cell r="J43"/>
-          <cell r="K43"/>
-          <cell r="L43"/>
-          <cell r="M43"/>
-          <cell r="N43"/>
-          <cell r="O43"/>
-          <cell r="P43"/>
-          <cell r="Q43"/>
-          <cell r="R43"/>
-          <cell r="S43"/>
-          <cell r="T43"/>
-          <cell r="U43"/>
-          <cell r="V43"/>
-          <cell r="W43"/>
-          <cell r="X43"/>
           <cell r="Y43">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -5979,27 +5511,6 @@
           <cell r="C44">
             <v>43</v>
           </cell>
-          <cell r="D44"/>
-          <cell r="E44"/>
-          <cell r="F44"/>
-          <cell r="G44"/>
-          <cell r="H44"/>
-          <cell r="I44"/>
-          <cell r="J44"/>
-          <cell r="K44"/>
-          <cell r="L44"/>
-          <cell r="M44"/>
-          <cell r="N44"/>
-          <cell r="O44"/>
-          <cell r="P44"/>
-          <cell r="Q44"/>
-          <cell r="R44"/>
-          <cell r="S44"/>
-          <cell r="T44"/>
-          <cell r="U44"/>
-          <cell r="V44"/>
-          <cell r="W44"/>
-          <cell r="X44"/>
           <cell r="Y44">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -6080,29 +5591,6 @@
           <cell r="A45" t="str">
             <v>REF</v>
           </cell>
-          <cell r="B45"/>
-          <cell r="C45"/>
-          <cell r="D45"/>
-          <cell r="E45"/>
-          <cell r="F45"/>
-          <cell r="G45"/>
-          <cell r="H45"/>
-          <cell r="I45"/>
-          <cell r="J45"/>
-          <cell r="K45"/>
-          <cell r="L45"/>
-          <cell r="M45"/>
-          <cell r="N45"/>
-          <cell r="O45"/>
-          <cell r="P45"/>
-          <cell r="Q45"/>
-          <cell r="R45"/>
-          <cell r="S45"/>
-          <cell r="T45"/>
-          <cell r="U45"/>
-          <cell r="V45"/>
-          <cell r="W45"/>
-          <cell r="X45"/>
           <cell r="Y45">
             <v>-8.6999999999999994E-3</v>
           </cell>
@@ -6157,11 +5645,6 @@
           <cell r="AP45">
             <v>131.1</v>
           </cell>
-          <cell r="AQ45"/>
-          <cell r="AR45"/>
-          <cell r="AS45"/>
-          <cell r="AT45"/>
-          <cell r="AU45"/>
           <cell r="AV45">
             <v>0</v>
           </cell>
@@ -6503,7 +5986,7 @@
   <dimension ref="A1:AZ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6677,7 +6160,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="7">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E2" s="7">
         <v>2E-3</v>
@@ -6767,7 +6250,7 @@
         <v>6826.5</v>
       </c>
       <c r="AH2" s="7">
-        <v>-271.12892991402197</v>
+        <v>-320</v>
       </c>
       <c r="AI2" s="7">
         <v>13.131104586741001</v>
@@ -7151,7 +6634,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="7">
-        <v>2.1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="7">
         <v>2E-3</v>
@@ -7241,7 +6724,7 @@
         <v>6826.5</v>
       </c>
       <c r="AH5" s="7">
-        <v>-271.12892991402197</v>
+        <v>-320</v>
       </c>
       <c r="AI5" s="7">
         <v>8.7200000000000006</v>

</xml_diff>

<commit_message>
Fix Simulink model from previous commit
</commit_message>
<xml_diff>
--- a/4_Node_Heart_Network_Example.xlsx
+++ b/4_Node_Heart_Network_Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfen801\HeartModelPub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA71B3A-B22E-452D-90F2-D7791B84A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04725694-6D68-4F4D-B466-2F81BE630B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{CE794E2E-EB70-449E-A900-ACEA4681AAAE}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{CE794E2E-EB70-449E-A900-ACEA4681AAAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Node" sheetId="1" r:id="rId1"/>
@@ -5985,7 +5985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09EE518-A6B0-4237-BA56-0ADD842FBD35}">
   <dimension ref="A1:AZ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -6791,8 +6791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D028EE44-7DA0-4D5B-B019-D6C46FBDD67D}">
   <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6888,7 +6888,7 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -6903,7 +6903,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -6963,7 +6963,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -6978,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="K3">
         <v>1</v>

</xml_diff>

<commit_message>
Set up sustained reentry circuit
</commit_message>
<xml_diff>
--- a/4_Node_Heart_Network_Example.xlsx
+++ b/4_Node_Heart_Network_Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfen801\HeartModelPub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04725694-6D68-4F4D-B466-2F81BE630B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9578D859-AFB0-471B-A60A-0F330E32BC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{CE794E2E-EB70-449E-A900-ACEA4681AAAE}"/>
   </bookViews>
@@ -6792,7 +6792,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6888,7 +6888,7 @@
         <v>3</v>
       </c>
       <c r="E2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -6903,7 +6903,7 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -6963,7 +6963,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -6978,7 +6978,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -7038,7 +7038,7 @@
         <v>4</v>
       </c>
       <c r="E4">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -7053,7 +7053,7 @@
         <v>10.99</v>
       </c>
       <c r="J4">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -7113,7 +7113,7 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -7128,7 +7128,7 @@
         <v>10.99</v>
       </c>
       <c r="J5">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="K5">
         <v>1</v>

</xml_diff>